<commit_message>
debug messaegs, at commands logs
</commit_message>
<xml_diff>
--- a/thesis/Design_vendor_tests.xlsx
+++ b/thesis/Design_vendor_tests.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
-    <sheet name="4x4x4" sheetId="3" r:id="rId2"/>
-    <sheet name="Tests" sheetId="2" r:id="rId3"/>
+    <sheet name="eDRX" sheetId="5" r:id="rId2"/>
+    <sheet name="4x4x4" sheetId="3" r:id="rId3"/>
     <sheet name="Manufacturers" sheetId="4" r:id="rId4"/>
+    <sheet name="Tests" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="172">
   <si>
     <t>Ublox</t>
   </si>
@@ -441,6 +442,111 @@
   </si>
   <si>
     <t>SierraWireless</t>
+  </si>
+  <si>
+    <t>+CEREG: 5,1,"8CA7","28C465",7,,,"00010000","00101010"</t>
+  </si>
+  <si>
+    <t>&gt; +NPTWEDRXS: 5,"0000","0000"</t>
+  </si>
+  <si>
+    <t>&gt; +CEREG: 5,1,"8CA7","28C465",7,,,"00010000","00101010"</t>
+  </si>
+  <si>
+    <t>Active T3324: 32 seconds, Periodic T3412: 10 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; </t>
+  </si>
+  <si>
+    <t>&gt; Active T3324: 32 seconds, Periodic T3412: 10 hours</t>
+  </si>
+  <si>
+    <t>&gt; +NPTWEDRXS: 5,"1001","0010"</t>
+  </si>
+  <si>
+    <t>NW provided eDRX value: 81.92 seconds, Paging Time Window: 2.56 seconds</t>
+  </si>
+  <si>
+    <t>&gt; +CEREG: 5,1,"8CA7","28C465",7,,,"00010110","00101010"</t>
+  </si>
+  <si>
+    <t>Active T3324: 44 seconds, Periodic T3412: 10 hours</t>
+  </si>
+  <si>
+    <t>&gt; +NPTWEDRXS: 5,"0000","0010"</t>
+  </si>
+  <si>
+    <t>NW provided eDRX value: 40.96 seconds, Paging Time Window: 2.56 seconds</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>eDRX value: 40.96 seconds, Paging Time Window: 2.56 seconds</t>
+  </si>
+  <si>
+    <t>eDRX value: 10.24 seconds, Paging Time Window: 5.12 seconds</t>
+  </si>
+  <si>
+    <t>eDRX value: 10.24 seconds, Paging Time Window: 2.56 seconds</t>
+  </si>
+  <si>
+    <t>&gt; +NPTWEDRXP: 5,"0000","0011","0011","0000"</t>
+  </si>
+  <si>
+    <t>&gt; +NPTWEDRXS: 5,"0000","0100"</t>
+  </si>
+  <si>
+    <t>&gt; +CEREG: 5,1,"8CA7","28C464",7,,,"00010000","00101010"</t>
+  </si>
+  <si>
+    <t>&gt; +NPTWEDRXP: 5,"0000","0101","0101","0000</t>
+  </si>
+  <si>
+    <t>NW provided eDRX value: 327.68 seconds, Paging Time Window: 2.56 seconds</t>
+  </si>
+  <si>
+    <t>+CEREG: 5,1,"8CA7","28C465",7,,,"00100010","00101010"</t>
+  </si>
+  <si>
+    <t>&gt; Active T3324: 2 minutes, Periodic T3412: 10 hours</t>
+  </si>
+  <si>
+    <t>&gt; +NPTWEDRXP: 5,"0000","0110","0010","0000</t>
+  </si>
+  <si>
+    <t>&gt; +NPTWEDRXS: 5,"0000","0111"</t>
+  </si>
+  <si>
+    <t>eDRX value: 1310.72 seconds, Paging Time Window: 2.56 seconds</t>
+  </si>
+  <si>
+    <t>eDRX value: 163.84 seconds, Paging Time Window: 2.56 seconds</t>
+  </si>
+  <si>
+    <t>&gt; +NPTWEDRXS: 5,"0000","1000"</t>
+  </si>
+  <si>
+    <t>eDRX value: 1966.08 seconds, Paging Time Window: 2.56 seconds</t>
+  </si>
+  <si>
+    <t>at+cops=2</t>
+  </si>
+  <si>
+    <t>at+cops=0</t>
+  </si>
+  <si>
+    <t>&gt; +CPSMS: 1,,,"01000001","00000101"</t>
+  </si>
+  <si>
+    <t>Active T3324: 10 seconds, Periodic T3412: 10 hours</t>
   </si>
 </sst>
 </file>
@@ -522,21 +628,21 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -948,6 +1054,316 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E10:T63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="10" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="Q10" t="s">
+        <v>149</v>
+      </c>
+      <c r="R10" t="s">
+        <v>150</v>
+      </c>
+      <c r="S10" t="s">
+        <v>151</v>
+      </c>
+      <c r="T10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>12</v>
+      </c>
+      <c r="S12">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="13" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>12</v>
+      </c>
+      <c r="S17">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="18" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q22">
+        <v>24</v>
+      </c>
+      <c r="R22">
+        <v>2</v>
+      </c>
+      <c r="S22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
+      <c r="R26">
+        <v>2</v>
+      </c>
+      <c r="S26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q32">
+        <v>28</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q36">
+        <v>23</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q41">
+        <v>23</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>163</v>
+      </c>
+      <c r="T46">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>166</v>
+      </c>
+      <c r="T51">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="57" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>171</v>
+      </c>
+      <c r="T62">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D7:U29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -960,7 +1376,7 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>103</v>
       </c>
       <c r="E7" t="s">
@@ -975,10 +1391,10 @@
       <c r="H7" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="L7" s="8"/>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
@@ -1045,7 +1461,7 @@
       </c>
     </row>
     <row r="13" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>104</v>
       </c>
       <c r="E13" t="s">
@@ -1084,14 +1500,14 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4" t="s">
+      <c r="S16" s="10"/>
+      <c r="T16" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="U16" s="4"/>
+      <c r="U16" s="10"/>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
@@ -1134,7 +1550,7 @@
       </c>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>105</v>
       </c>
       <c r="E19" t="s">
@@ -1183,7 +1599,7 @@
       </c>
     </row>
     <row r="25" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>106</v>
       </c>
       <c r="E25" t="s">
@@ -1242,7 +1658,184 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E8:K24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="7"/>
+    <col min="5" max="5" width="18.7109375" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E8" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7">
+        <v>5</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E10" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E11" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="7">
+        <v>6</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E12" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="5:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E14" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E16" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E18" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F23" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="7">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A8:G56"/>
   <sheetViews>
@@ -1445,7 +2038,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C29" t="s">
@@ -1462,11 +2055,11 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
+      <c r="B30" s="10"/>
       <c r="C30" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>65</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1477,11 +2070,11 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
+      <c r="B31" s="10"/>
       <c r="C31" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -1495,11 +2088,11 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="4"/>
+      <c r="B32" s="10"/>
       <c r="C32" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>70</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -1513,11 +2106,11 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
+      <c r="B33" s="10"/>
       <c r="C33" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E33" s="1" t="s">
@@ -1528,11 +2121,11 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
+      <c r="B34" s="10"/>
       <c r="C34" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="4" t="s">
         <v>54</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -1543,11 +2136,11 @@
       </c>
     </row>
     <row r="35" spans="2:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
+      <c r="B35" s="10"/>
       <c r="C35" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -1556,16 +2149,16 @@
       <c r="F35" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="G35" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="4"/>
+      <c r="B36" s="10"/>
       <c r="C36" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>72</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -1576,11 +2169,11 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="4"/>
+      <c r="B37" s="10"/>
       <c r="C37" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>73</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -1591,11 +2184,11 @@
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="4"/>
+      <c r="B38" s="10"/>
       <c r="C38" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E38" s="2" t="s">
@@ -1609,11 +2202,11 @@
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="4"/>
+      <c r="B39" s="10"/>
       <c r="C39" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -1641,7 +2234,7 @@
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C41" t="s">
@@ -1649,55 +2242,55 @@
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
+      <c r="B42" s="10"/>
       <c r="C42" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="4"/>
+      <c r="B43" s="10"/>
       <c r="C43" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="4"/>
+      <c r="B44" s="10"/>
       <c r="C44" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="4"/>
+      <c r="B45" s="10"/>
       <c r="C45" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="4"/>
+      <c r="B46" s="10"/>
       <c r="C46" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="4"/>
+      <c r="B47" s="10"/>
       <c r="C47" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="4"/>
+      <c r="B48" s="10"/>
       <c r="C48" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="4"/>
+      <c r="B49" s="10"/>
       <c r="C49" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="4"/>
+      <c r="B50" s="10"/>
       <c r="C50" t="s">
         <v>84</v>
       </c>
@@ -1709,7 +2302,7 @@
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C51" t="s">
@@ -1717,19 +2310,19 @@
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="4"/>
+      <c r="B52" s="10"/>
       <c r="C52" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="4"/>
+      <c r="B53" s="10"/>
       <c r="C53" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="4"/>
+      <c r="B54" s="10"/>
       <c r="C54" t="s">
         <v>89</v>
       </c>
@@ -1783,181 +2376,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E8:K24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8:K14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="9.140625" style="9"/>
-    <col min="5" max="5" width="18.7109375" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E8" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E9" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="9">
-        <v>5</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E10" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F10" s="9">
-        <v>2</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E11" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F11" s="9">
-        <v>6</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E12" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E13" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="9">
-        <v>1</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="5:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="E14" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="F14" s="9">
-        <v>2</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E16" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="F16" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F17" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="5:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="E18" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F18" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="F19" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="F20" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="F21" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="F22" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E23" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="F23" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="F24" s="9">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
notebook. edge. empty cops ,,
</commit_message>
<xml_diff>
--- a/thesis/Design_vendor_tests.xlsx
+++ b/thesis/Design_vendor_tests.xlsx
@@ -19,6 +19,7 @@
     <sheet name="Tests" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1056,7 +1057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E10:T63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
@@ -1739,7 +1740,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="5:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E14" s="8" t="s">
         <v>125</v>
       </c>
@@ -1774,7 +1775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="5:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:6" ht="30" x14ac:dyDescent="0.25">
       <c r="E18" s="8" t="s">
         <v>128</v>
       </c>

</xml_diff>